<commit_message>
Helpersheet: Add manual ref in morph comp of data helper spreadsheet
</commit_message>
<xml_diff>
--- a/Helper_Spreadsheets/SS_330_data_helper.xlsx
+++ b/Helper_Spreadsheets/SS_330_data_helper.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\Documents\vlab\helper_spreadsheet_update\update_to_3.30.14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\Documents\Stock_Synthesis\vlab_repo\SS_documentation\ss_documentation\Helper_Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2937,13 +2937,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>161924</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>171449</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2952,8 +2952,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7477124" y="466725"/>
-          <a:ext cx="3667125" cy="1304926"/>
+          <a:off x="7477124" y="466724"/>
+          <a:ext cx="3667125" cy="1724025"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3018,8 +3018,20 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> match the number of biological morphs in the control file.</a:t>
+            <a:t> match the number of biological morphs in the control file. For more information, see the </a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0" smtClean="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Stock (Morph) Composition Data section of the user manual.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" baseline="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3318,7 +3330,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3754,7 +3766,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3947,8 +3961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFB262"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E271" sqref="E271"/>
+    <sheetView topLeftCell="A225" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F256" sqref="F256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
#80117: document mean center/zscore options for env data in helper sheets
</commit_message>
<xml_diff>
--- a/Helper_Spreadsheets/SS_330_data_helper.xlsx
+++ b/Helper_Spreadsheets/SS_330_data_helper.xlsx
@@ -295,7 +295,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4451" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4453" uniqueCount="262">
   <si>
     <t>#_months/season</t>
   </si>
@@ -1075,6 +1075,12 @@
   </si>
   <si>
     <t>ENDDATA</t>
+  </si>
+  <si>
+    <t># this subtracts the mean from the data for variable 3</t>
+  </si>
+  <si>
+    <t># this zscores the data for variable 2</t>
   </si>
 </sst>
 </file>
@@ -3329,9 +3335,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3961,7 +3965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFB262"/>
   <sheetViews>
-    <sheetView topLeftCell="A225" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A240" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F256" sqref="F256"/>
     </sheetView>
   </sheetViews>
@@ -52528,20 +52532,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>29</v>
@@ -52549,8 +52555,12 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -52562,8 +52572,12 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1980</v>
       </c>
@@ -52575,8 +52589,12 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1981</v>
       </c>
@@ -52588,8 +52606,12 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>1982</v>
       </c>
@@ -52601,8 +52623,12 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>1983</v>
       </c>
@@ -52614,8 +52640,12 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>1984</v>
       </c>
@@ -52627,8 +52657,12 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>1980</v>
       </c>
@@ -52640,8 +52674,12 @@
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>1981</v>
       </c>
@@ -52653,8 +52691,12 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>1982</v>
       </c>
@@ -52666,8 +52708,12 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>1983</v>
       </c>
@@ -52679,8 +52725,12 @@
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>1984</v>
       </c>
@@ -52692,21 +52742,152 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
+        <v>1980</v>
+      </c>
+      <c r="B14" s="7">
+        <v>3</v>
+      </c>
+      <c r="C14" s="7">
+        <v>-0.1</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>1981</v>
+      </c>
+      <c r="B15" s="7">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>1982</v>
+      </c>
+      <c r="B16" s="7">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>1983</v>
+      </c>
+      <c r="B17" s="7">
+        <v>3</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>1984</v>
+      </c>
+      <c r="B18" s="7">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7">
+        <v>-0.2</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>-1</v>
+      </c>
+      <c r="B19" s="7">
+        <v>2</v>
+      </c>
+      <c r="C19" s="7">
+        <v>1</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>-2</v>
+      </c>
+      <c r="B20" s="7">
+        <v>3</v>
+      </c>
+      <c r="C20" s="7">
+        <v>1</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>260</v>
+      </c>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="57"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>-9999</v>
       </c>
-      <c r="B14" s="7">
-        <v>1</v>
-      </c>
-      <c r="C14" s="7">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="B21" s="7">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7">
+        <v>1</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
helper spreadsheets, #16: update equilibirium catch details
</commit_message>
<xml_diff>
--- a/Helper_Spreadsheets/SS_330_data_helper.xlsx
+++ b/Helper_Spreadsheets/SS_330_data_helper.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\Documents\Stock_Synthesis\vlab_repo\SS_documentation\ss_documentation\Helper_Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\Documents\Stock_Synthesis\nmfs-stock-synthesis-repos\ss-documentation\Helper_Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -645,9 +645,6 @@
     <t>#Catch_SE</t>
   </si>
   <si>
-    <t># -999 allows for initial equilibrium catch by fleet</t>
-  </si>
-  <si>
     <t># -9999 indicates the end of catch records to be read</t>
   </si>
   <si>
@@ -1109,6 +1106,9 @@
   <si>
     <t>See Control helper spreadsheet or SS manual for details on how to use DM weighting</t>
   </si>
+  <si>
+    <t xml:space="preserve"># -999 allows for initial equilibrium catch by fleet and season; If there is non-zero equilibrium catch, then a parameter line (for each fleet/season with non-zero catch) in the initial F section of the control files is required. See the initial fishing mortality section of SS user manual and the F section of control helper spreadsheet for more details. </t>
+  </si>
 </sst>
 </file>
 
@@ -1398,7 +1398,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1523,6 +1523,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -2082,16 +2085,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>174625</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2100,8 +2103,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5016500" y="6350000"/>
-          <a:ext cx="4025900" cy="1038225"/>
+          <a:off x="3860800" y="6791325"/>
+          <a:ext cx="4064000" cy="1038225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2148,7 +2151,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> number of years with catch is longer needs to be specified.  Version 3.30 requires that catches be inputted in a list by fleet/survey.  The value of -9999 indicates the end of catch records to be read</a:t>
+            <a:t> number of years with catch is longer needs to be specified.  Version 3.30 requires that catches are input in a list by fleet/survey.  The value of -9999 indicates the end of catch records to be read</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -3362,9 +3365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3384,15 +3385,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="66" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3400,7 +3401,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3413,12 +3414,12 @@
         <v>83</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B9" s="17" t="s">
         <v>84</v>
@@ -3426,40 +3427,40 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>225</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>87</v>
@@ -3467,7 +3468,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B17" s="17" t="s">
         <v>88</v>
@@ -3475,7 +3476,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B18" s="17" t="s">
         <v>89</v>
@@ -3483,7 +3484,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>90</v>
@@ -3546,7 +3547,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -3624,25 +3625,25 @@
         <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>65</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -3717,7 +3718,7 @@
         <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>54</v>
@@ -3807,7 +3808,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -3833,7 +3834,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -3851,7 +3852,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -3869,7 +3870,7 @@
         <v>1E-3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -3887,7 +3888,7 @@
         <v>49</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>50</v>
@@ -3903,7 +3904,7 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I7" s="58"/>
       <c r="J7" s="58"/>
@@ -3968,7 +3969,7 @@
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="40" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B10" s="41"/>
       <c r="C10" s="41"/>
@@ -3994,8 +3995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFB263"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L108" sqref="L108"/>
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4006,7 +4007,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -4057,7 +4058,7 @@
         <v>1971</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -4083,7 +4084,7 @@
         <v>2001</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -4109,7 +4110,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -4187,7 +4188,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -4213,7 +4214,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -4338,7 +4339,7 @@
     </row>
     <row r="14" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -4410,7 +4411,7 @@
     </row>
     <row r="17" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -4434,7 +4435,7 @@
     </row>
     <row r="18" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4458,22 +4459,22 @@
     </row>
     <row r="19" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -4586,7 +4587,7 @@
       </c>
       <c r="H22" s="2"/>
       <c r="I22" s="65" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J22" s="63"/>
       <c r="K22" s="64"/>
@@ -4602,7 +4603,7 @@
     </row>
     <row r="23" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -4626,7 +4627,7 @@
     </row>
     <row r="24" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -4650,7 +4651,7 @@
     </row>
     <row r="25" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -4674,7 +4675,7 @@
     </row>
     <row r="26" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -4698,7 +4699,7 @@
     </row>
     <row r="27" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -4722,7 +4723,7 @@
     </row>
     <row r="28" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -4746,7 +4747,7 @@
     </row>
     <row r="29" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -4770,7 +4771,7 @@
     </row>
     <row r="30" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -4794,7 +4795,7 @@
     </row>
     <row r="31" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -4848,7 +4849,7 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>-999</v>
       </c>
@@ -4859,28 +4860,28 @@
         <v>1</v>
       </c>
       <c r="D33" s="7">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E33" s="7">
         <v>0.01</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
+      <c r="F33" s="81" t="s">
+        <v>270</v>
+      </c>
+      <c r="G33" s="81"/>
+      <c r="H33" s="81"/>
+      <c r="I33" s="81"/>
+      <c r="J33" s="81"/>
+      <c r="K33" s="81"/>
+      <c r="L33" s="81"/>
+      <c r="M33" s="81"/>
+      <c r="N33" s="81"/>
+      <c r="O33" s="81"/>
+      <c r="P33" s="81"/>
+      <c r="Q33" s="81"/>
+      <c r="R33" s="81"/>
+      <c r="S33" s="81"/>
+      <c r="T33" s="81"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
@@ -4898,21 +4899,21 @@
       <c r="E34" s="7">
         <v>0.01</v>
       </c>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="2"/>
+      <c r="F34" s="81"/>
+      <c r="G34" s="81"/>
+      <c r="H34" s="81"/>
+      <c r="I34" s="81"/>
+      <c r="J34" s="81"/>
+      <c r="K34" s="81"/>
+      <c r="L34" s="81"/>
+      <c r="M34" s="81"/>
+      <c r="N34" s="81"/>
+      <c r="O34" s="81"/>
+      <c r="P34" s="81"/>
+      <c r="Q34" s="81"/>
+      <c r="R34" s="81"/>
+      <c r="S34" s="81"/>
+      <c r="T34" s="81"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
@@ -4930,21 +4931,21 @@
       <c r="E35" s="7">
         <v>0.01</v>
       </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="2"/>
+      <c r="F35" s="81"/>
+      <c r="G35" s="81"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="81"/>
+      <c r="J35" s="81"/>
+      <c r="K35" s="81"/>
+      <c r="L35" s="81"/>
+      <c r="M35" s="81"/>
+      <c r="N35" s="81"/>
+      <c r="O35" s="81"/>
+      <c r="P35" s="81"/>
+      <c r="Q35" s="81"/>
+      <c r="R35" s="81"/>
+      <c r="S35" s="81"/>
+      <c r="T35" s="81"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
@@ -5892,7 +5893,7 @@
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="67" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H65" s="68"/>
       <c r="I65" s="68"/>
@@ -5910,7 +5911,7 @@
     </row>
     <row r="66" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -5994,7 +5995,7 @@
     </row>
     <row r="69" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -6027,7 +6028,7 @@
         <v>11</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
@@ -6066,7 +6067,7 @@
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="65" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J71" s="63"/>
       <c r="K71" s="63"/>
@@ -6195,7 +6196,7 @@
         <v>0.3</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
@@ -6229,7 +6230,7 @@
         <v>0.3</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
@@ -6263,7 +6264,7 @@
         <v>0.3</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
@@ -6297,7 +6298,7 @@
         <v>0.3</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
@@ -6331,7 +6332,7 @@
         <v>0.3</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
@@ -6365,7 +6366,7 @@
         <v>0.3</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
@@ -6399,7 +6400,7 @@
         <v>0.3</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
@@ -6433,7 +6434,7 @@
         <v>0.3</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
@@ -6467,7 +6468,7 @@
         <v>0.3</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
@@ -6501,7 +6502,7 @@
         <v>0.7</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
@@ -6535,7 +6536,7 @@
         <v>0.7</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
@@ -6569,7 +6570,7 @@
         <v>0.7</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
@@ -6603,7 +6604,7 @@
         <v>0.7</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
@@ -6637,7 +6638,7 @@
         <v>0.7</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
@@ -6671,7 +6672,7 @@
         <v>0.7</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
@@ -6705,7 +6706,7 @@
         <v>0.7</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
@@ -6739,7 +6740,7 @@
         <v>0.7</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
@@ -6773,7 +6774,7 @@
         <v>0.7</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
@@ -6807,7 +6808,7 @@
         <v>0.7</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
@@ -6841,7 +6842,7 @@
         <v>0.7</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
@@ -6875,7 +6876,7 @@
         <v>0.7</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
@@ -6909,7 +6910,7 @@
         <v>1</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
@@ -6928,7 +6929,7 @@
     </row>
     <row r="97" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -6964,7 +6965,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
       <c r="I98" s="65" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J98" s="63"/>
       <c r="K98" s="63"/>
@@ -6980,7 +6981,7 @@
     </row>
     <row r="99" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -7007,7 +7008,7 @@
         <v>0</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
@@ -7016,7 +7017,7 @@
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="65" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J100" s="63"/>
       <c r="K100" s="63"/>
@@ -7032,7 +7033,7 @@
     </row>
     <row r="101" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -7056,7 +7057,7 @@
     </row>
     <row r="102" spans="1:23" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B102" s="63"/>
       <c r="C102" s="63"/>
@@ -7083,7 +7084,7 @@
     </row>
     <row r="103" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -7214,7 +7215,7 @@
         <v>1</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
@@ -7333,7 +7334,7 @@
     </row>
     <row r="113" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -7357,7 +7358,7 @@
     </row>
     <row r="114" spans="1:56" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -7381,14 +7382,14 @@
     </row>
     <row r="115" spans="1:56" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="60" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G115" s="63"/>
       <c r="H115" s="63"/>
@@ -7407,7 +7408,7 @@
     </row>
     <row r="116" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -7431,25 +7432,25 @@
     </row>
     <row r="117" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="C117" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="D117" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="D117" s="2" t="s">
+      <c r="E117" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="E117" s="2" t="s">
+      <c r="F117" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="F117" s="2" t="s">
+      <c r="G117" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="G117" s="2" t="s">
-        <v>268</v>
       </c>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
@@ -7711,13 +7712,13 @@
         <v>17</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>21</v>
@@ -16452,7 +16453,7 @@
     </row>
     <row r="176" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -16903,7 +16904,7 @@
     </row>
     <row r="185" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B185" s="6"/>
       <c r="C185" s="6"/>
@@ -17204,7 +17205,7 @@
     </row>
     <row r="188" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B188" s="6"/>
       <c r="C188" s="6"/>
@@ -17505,7 +17506,7 @@
     </row>
     <row r="191" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
@@ -17740,7 +17741,7 @@
     </row>
     <row r="196" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
@@ -17787,7 +17788,7 @@
     </row>
     <row r="197" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
@@ -17834,7 +17835,7 @@
     </row>
     <row r="198" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
@@ -17881,7 +17882,7 @@
     </row>
     <row r="199" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
@@ -18259,13 +18260,13 @@
         <v>17</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D206" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E206" s="2" t="s">
         <v>21</v>
@@ -23692,7 +23693,7 @@
     </row>
     <row r="248" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
@@ -23749,7 +23750,7 @@
       <c r="D249" s="2"/>
       <c r="E249" s="2"/>
       <c r="F249" s="65" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G249" s="63"/>
       <c r="H249" s="64"/>
@@ -23792,7 +23793,7 @@
     </row>
     <row r="250" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
@@ -23849,7 +23850,7 @@
       <c r="D251" s="2"/>
       <c r="E251" s="2"/>
       <c r="F251" s="65" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G251" s="63"/>
       <c r="H251" s="64"/>
@@ -23892,7 +23893,7 @@
     </row>
     <row r="252" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
@@ -23949,7 +23950,7 @@
       <c r="D253" s="2"/>
       <c r="E253" s="2"/>
       <c r="F253" s="65" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G253" s="63"/>
       <c r="H253" s="63"/>
@@ -23992,7 +23993,7 @@
     </row>
     <row r="254" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
@@ -24049,7 +24050,7 @@
       <c r="D255" s="2"/>
       <c r="E255" s="2"/>
       <c r="F255" s="65" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G255" s="63"/>
       <c r="H255" s="64"/>
@@ -24091,7 +24092,7 @@
     </row>
     <row r="256" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
@@ -24147,7 +24148,7 @@
       <c r="D257" s="2"/>
       <c r="E257" s="2"/>
       <c r="F257" s="65" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G257" s="63"/>
       <c r="H257" s="64"/>
@@ -24189,7 +24190,7 @@
     </row>
     <row r="258" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
@@ -24239,13 +24240,13 @@
         <v>0</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C259" s="2"/>
       <c r="D259" s="2"/>
       <c r="E259" s="2"/>
       <c r="F259" s="62" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G259" s="63"/>
       <c r="H259" s="63"/>
@@ -48672,7 +48673,7 @@
     </row>
     <row r="260" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" x14ac:dyDescent="0.25">
       <c r="A260" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
@@ -48813,7 +48814,7 @@
     </row>
     <row r="263" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
@@ -48859,6 +48860,9 @@
       <c r="AQ263" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F33:T35"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="F249" location="'Mean Size-at-Age'!A1" display="See the Mean Size-at-Age tab"/>
     <hyperlink ref="F251" location="Environmental!A1" display="See the Environmental tab"/>
@@ -48887,7 +48891,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.35">
@@ -48934,7 +48938,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -48985,7 +48989,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -49002,7 +49006,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -49019,7 +49023,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -49187,10 +49191,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -49228,7 +49232,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -49247,7 +49251,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -49308,19 +49312,19 @@
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>40</v>
@@ -49343,7 +49347,7 @@
         <v>0.3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -49363,7 +49367,7 @@
         <v>0.3</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -49383,7 +49387,7 @@
         <v>0.3</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -49403,7 +49407,7 @@
         <v>0.3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -49423,7 +49427,7 @@
         <v>0.3</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -49443,7 +49447,7 @@
         <v>0.3</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -49463,7 +49467,7 @@
         <v>0.3</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -49483,7 +49487,7 @@
         <v>0.3</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -49503,7 +49507,7 @@
         <v>0.3</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -49523,7 +49527,7 @@
         <v>0.3</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -49543,7 +49547,7 @@
         <v>0.3</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -49563,7 +49567,7 @@
         <v>0.3</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -49583,7 +49587,7 @@
         <v>1E-3</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -49603,7 +49607,7 @@
         <v>1E-3</v>
       </c>
       <c r="F26" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -49629,7 +49633,7 @@
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.35">
@@ -49724,7 +49728,7 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -49752,7 +49756,7 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -49780,7 +49784,7 @@
     </row>
     <row r="9" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -49813,7 +49817,7 @@
     </row>
     <row r="10" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -49846,7 +49850,7 @@
     </row>
     <row r="11" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -49879,7 +49883,7 @@
     </row>
     <row r="12" spans="1:29" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -49912,17 +49916,17 @@
     </row>
     <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>176</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F13" s="41"/>
       <c r="G13" s="41"/>
@@ -49958,7 +49962,7 @@
         <v>104</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F14" s="41"/>
       <c r="G14" s="41"/>
@@ -50001,7 +50005,7 @@
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I15" s="45"/>
       <c r="J15" s="46"/>
@@ -50037,7 +50041,7 @@
         <v>0.3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -50075,7 +50079,7 @@
         <v>0.3</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -50113,7 +50117,7 @@
         <v>0.3</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -50151,7 +50155,7 @@
         <v>0.3</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
@@ -50178,7 +50182,7 @@
         <v>0.3</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -50205,7 +50209,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -50232,7 +50236,7 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -50244,7 +50248,7 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -50256,7 +50260,7 @@
     </row>
     <row r="29" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -50268,13 +50272,13 @@
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="72" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F30" s="73"/>
       <c r="G30" s="74"/>
@@ -50282,7 +50286,7 @@
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -50294,7 +50298,7 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -50306,13 +50310,13 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B33" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>176</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="75"/>
@@ -50377,7 +50381,7 @@
         <v>0.3</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -50399,7 +50403,7 @@
         <v>0.3</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -50421,7 +50425,7 @@
         <v>0.3</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
@@ -50443,7 +50447,7 @@
         <v>0.3</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -50465,7 +50469,7 @@
         <v>0.3</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
@@ -50487,7 +50491,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -50508,7 +50512,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -50520,7 +50524,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -50532,7 +50536,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -50544,7 +50548,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -50556,7 +50560,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -50568,7 +50572,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -50580,13 +50584,13 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="C53" s="4" t="s">
         <v>175</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>176</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -50651,7 +50655,7 @@
         <v>0.3</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
@@ -50673,7 +50677,7 @@
         <v>0.3</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -50695,7 +50699,7 @@
         <v>0.3</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -50717,7 +50721,7 @@
         <v>0.3</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -50739,7 +50743,7 @@
         <v>0.3</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -50761,7 +50765,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -50789,10 +50793,10 @@
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -50801,7 +50805,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -50821,7 +50825,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -50838,7 +50842,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -50848,7 +50852,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="48" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J8" s="49"/>
       <c r="K8" s="49"/>
@@ -50861,7 +50865,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>54</v>
@@ -50870,19 +50874,19 @@
         <v>51</v>
       </c>
       <c r="E9" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>188</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>40</v>
       </c>
       <c r="I9" s="51" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J9" s="52"/>
       <c r="K9" s="52"/>
@@ -50913,10 +50917,10 @@
         <v>0.32500000000000001</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I10" s="51" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J10" s="52"/>
       <c r="K10" s="52"/>
@@ -50947,10 +50951,10 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I11" s="54" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J11" s="55"/>
       <c r="K11" s="55"/>
@@ -50981,7 +50985,7 @@
         <v>0.17</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -51013,7 +51017,7 @@
         <v>0.16700000000000001</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -51045,7 +51049,7 @@
         <v>0.33700000000000002</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -51077,7 +51081,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -51102,10 +51106,10 @@
   <sheetData>
     <row r="1" spans="1:77" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:77" x14ac:dyDescent="0.25">
@@ -52586,7 +52590,7 @@
         <v>0</v>
       </c>
       <c r="BX11" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="BY11" s="2"/>
     </row>
@@ -52632,10 +52636,10 @@
         <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -52910,7 +52914,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="48" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E19" s="49"/>
       <c r="F19" s="49"/>
@@ -52929,7 +52933,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E20" s="41"/>
       <c r="F20" s="41"/>
@@ -52948,7 +52952,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -52973,7 +52977,7 @@
   <sheetData>
     <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
@@ -53370,7 +53374,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>54</v>
@@ -53565,7 +53569,7 @@
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>

</xml_diff>

<commit_message>
helper, #61: document predator fleet in helper spreadsheets
</commit_message>
<xml_diff>
--- a/Helper_Spreadsheets/SS_330_data_helper.xlsx
+++ b/Helper_Spreadsheets/SS_330_data_helper.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\Documents\Stock_Synthesis\nmfs-stock-synthesis-repos\ss-documentation\Helper_Spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kathryn.Doering\Documents\github_repos\ss-documentation\Helper_Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11955" windowHeight="7485"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11952" windowHeight="7488"/>
   </bookViews>
   <sheets>
     <sheet name="Index to Features" sheetId="7" r:id="rId1"/>
@@ -295,7 +295,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4461" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4462" uniqueCount="273">
   <si>
     <t>#_months/season</t>
   </si>
@@ -1109,6 +1109,12 @@
   <si>
     <t xml:space="preserve"># -999 allows for initial equilibrium catch by fleet and season; If there is non-zero equilibrium catch, then a parameter line (for each fleet/season with non-zero catch) in the initial F section of the control files is required. See the initial fishing mortality section of SS user manual and the F section of control helper spreadsheet for more details. </t>
   </si>
+  <si>
+    <t>#_fleet_type: 1=catch fleet; 2=bycatch only fleet; 3=survey; 4=predator as fleet (adds additional mortality without a fleet F)</t>
+  </si>
+  <si>
+    <t>NOTE: For each fleet that is designated as a predator (fleet type 4), a new parameter line is created in the mortality-growth (MGparm) section in the control file</t>
+  </si>
 </sst>
 </file>
 
@@ -1497,6 +1503,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1523,9 +1532,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3367,23 +3373,23 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" customWidth="1"/>
-    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="1" max="1" width="39.5546875" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="61"/>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:2" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:2" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="70" t="s">
         <v>92</v>
       </c>
       <c r="B3" s="71"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="66" t="s">
         <v>248</v>
       </c>
@@ -3391,12 +3397,12 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>81</v>
       </c>
@@ -3404,12 +3410,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>83</v>
       </c>
@@ -3417,7 +3423,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>223</v>
       </c>
@@ -3425,7 +3431,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>224</v>
       </c>
@@ -3433,32 +3439,32 @@
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="17" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="17" t="s">
         <v>231</v>
       </c>
@@ -3466,7 +3472,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>232</v>
       </c>
@@ -3474,7 +3480,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>233</v>
       </c>
@@ -3482,7 +3488,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>234</v>
       </c>
@@ -3490,7 +3496,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>86</v>
       </c>
@@ -3540,17 +3546,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -3564,7 +3570,7 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -3578,7 +3584,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -3592,7 +3598,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>0</v>
       </c>
@@ -3606,7 +3612,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>30</v>
       </c>
@@ -3620,7 +3626,7 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>67</v>
       </c>
@@ -3646,7 +3652,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>1</v>
       </c>
@@ -3672,7 +3678,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>2</v>
       </c>
@@ -3698,7 +3704,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>70</v>
       </c>
@@ -3710,7 +3716,7 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>67</v>
       </c>
@@ -3730,7 +3736,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>1</v>
       </c>
@@ -3750,7 +3756,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>1</v>
       </c>
@@ -3770,7 +3776,7 @@
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>1</v>
       </c>
@@ -3804,14 +3810,14 @@
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -3829,7 +3835,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -3847,7 +3853,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -3865,7 +3871,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:14" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>1E-3</v>
       </c>
@@ -3883,7 +3889,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>49</v>
       </c>
@@ -3911,7 +3917,7 @@
       <c r="K7" s="58"/>
       <c r="L7" s="59"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>2001</v>
       </c>
@@ -3939,7 +3945,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>2002</v>
       </c>
@@ -3967,7 +3973,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="40" t="s">
         <v>220</v>
       </c>
@@ -3999,13 +4005,13 @@
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>249</v>
       </c>
@@ -4029,7 +4035,7 @@
       <c r="S1" s="2"/>
       <c r="T1" s="2"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>75</v>
       </c>
@@ -4053,7 +4059,7 @@
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>1971</v>
       </c>
@@ -4079,7 +4085,7 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>2001</v>
       </c>
@@ -4105,7 +4111,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>1</v>
       </c>
@@ -4131,7 +4137,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>12</v>
       </c>
@@ -4157,7 +4163,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>2</v>
       </c>
@@ -4183,7 +4189,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>1</v>
       </c>
@@ -4209,7 +4215,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>2</v>
       </c>
@@ -4235,7 +4241,7 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>40</v>
       </c>
@@ -4261,7 +4267,7 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>1</v>
       </c>
@@ -4287,7 +4293,7 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>3</v>
       </c>
@@ -4313,7 +4319,7 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>95</v>
       </c>
@@ -4337,7 +4343,7 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>139</v>
       </c>
@@ -4361,7 +4367,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="1:20" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>96</v>
       </c>
@@ -4385,7 +4391,7 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:20" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>97</v>
       </c>
@@ -4409,7 +4415,7 @@
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>120</v>
       </c>
@@ -4433,7 +4439,7 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>121</v>
       </c>
@@ -4457,7 +4463,7 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
     </row>
-    <row r="19" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>134</v>
       </c>
@@ -4491,7 +4497,7 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>1</v>
       </c>
@@ -4527,7 +4533,7 @@
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
     </row>
-    <row r="21" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>3</v>
       </c>
@@ -4563,7 +4569,7 @@
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
     </row>
-    <row r="22" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7">
         <v>3</v>
       </c>
@@ -4601,7 +4607,7 @@
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
     </row>
-    <row r="23" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>140</v>
       </c>
@@ -4625,7 +4631,7 @@
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
     </row>
-    <row r="24" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>122</v>
       </c>
@@ -4649,7 +4655,7 @@
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
     </row>
-    <row r="25" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>123</v>
       </c>
@@ -4673,7 +4679,7 @@
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
     </row>
-    <row r="26" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>124</v>
       </c>
@@ -4697,7 +4703,7 @@
       <c r="S26" s="2"/>
       <c r="T26" s="2"/>
     </row>
-    <row r="27" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>125</v>
       </c>
@@ -4721,7 +4727,7 @@
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
     </row>
-    <row r="28" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>126</v>
       </c>
@@ -4745,7 +4751,7 @@
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
     </row>
-    <row r="29" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>127</v>
       </c>
@@ -4769,7 +4775,7 @@
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
     </row>
-    <row r="30" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>128</v>
       </c>
@@ -4793,7 +4799,7 @@
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
     </row>
-    <row r="31" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>129</v>
       </c>
@@ -4817,7 +4823,7 @@
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
     </row>
-    <row r="32" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>49</v>
       </c>
@@ -4849,7 +4855,7 @@
       <c r="S32" s="2"/>
       <c r="T32" s="2"/>
     </row>
-    <row r="33" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>-999</v>
       </c>
@@ -4865,25 +4871,25 @@
       <c r="E33" s="7">
         <v>0.01</v>
       </c>
-      <c r="F33" s="81" t="s">
+      <c r="F33" s="72" t="s">
         <v>270</v>
       </c>
-      <c r="G33" s="81"/>
-      <c r="H33" s="81"/>
-      <c r="I33" s="81"/>
-      <c r="J33" s="81"/>
-      <c r="K33" s="81"/>
-      <c r="L33" s="81"/>
-      <c r="M33" s="81"/>
-      <c r="N33" s="81"/>
-      <c r="O33" s="81"/>
-      <c r="P33" s="81"/>
-      <c r="Q33" s="81"/>
-      <c r="R33" s="81"/>
-      <c r="S33" s="81"/>
-      <c r="T33" s="81"/>
+      <c r="G33" s="72"/>
+      <c r="H33" s="72"/>
+      <c r="I33" s="72"/>
+      <c r="J33" s="72"/>
+      <c r="K33" s="72"/>
+      <c r="L33" s="72"/>
+      <c r="M33" s="72"/>
+      <c r="N33" s="72"/>
+      <c r="O33" s="72"/>
+      <c r="P33" s="72"/>
+      <c r="Q33" s="72"/>
+      <c r="R33" s="72"/>
+      <c r="S33" s="72"/>
+      <c r="T33" s="72"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>1971</v>
       </c>
@@ -4899,23 +4905,23 @@
       <c r="E34" s="7">
         <v>0.01</v>
       </c>
-      <c r="F34" s="81"/>
-      <c r="G34" s="81"/>
-      <c r="H34" s="81"/>
-      <c r="I34" s="81"/>
-      <c r="J34" s="81"/>
-      <c r="K34" s="81"/>
-      <c r="L34" s="81"/>
-      <c r="M34" s="81"/>
-      <c r="N34" s="81"/>
-      <c r="O34" s="81"/>
-      <c r="P34" s="81"/>
-      <c r="Q34" s="81"/>
-      <c r="R34" s="81"/>
-      <c r="S34" s="81"/>
-      <c r="T34" s="81"/>
+      <c r="F34" s="72"/>
+      <c r="G34" s="72"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="72"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="72"/>
+      <c r="N34" s="72"/>
+      <c r="O34" s="72"/>
+      <c r="P34" s="72"/>
+      <c r="Q34" s="72"/>
+      <c r="R34" s="72"/>
+      <c r="S34" s="72"/>
+      <c r="T34" s="72"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>1972</v>
       </c>
@@ -4931,23 +4937,23 @@
       <c r="E35" s="7">
         <v>0.01</v>
       </c>
-      <c r="F35" s="81"/>
-      <c r="G35" s="81"/>
-      <c r="H35" s="81"/>
-      <c r="I35" s="81"/>
-      <c r="J35" s="81"/>
-      <c r="K35" s="81"/>
-      <c r="L35" s="81"/>
-      <c r="M35" s="81"/>
-      <c r="N35" s="81"/>
-      <c r="O35" s="81"/>
-      <c r="P35" s="81"/>
-      <c r="Q35" s="81"/>
-      <c r="R35" s="81"/>
-      <c r="S35" s="81"/>
-      <c r="T35" s="81"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+      <c r="H35" s="72"/>
+      <c r="I35" s="72"/>
+      <c r="J35" s="72"/>
+      <c r="K35" s="72"/>
+      <c r="L35" s="72"/>
+      <c r="M35" s="72"/>
+      <c r="N35" s="72"/>
+      <c r="O35" s="72"/>
+      <c r="P35" s="72"/>
+      <c r="Q35" s="72"/>
+      <c r="R35" s="72"/>
+      <c r="S35" s="72"/>
+      <c r="T35" s="72"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>1973</v>
       </c>
@@ -4979,7 +4985,7 @@
       <c r="S36" s="2"/>
       <c r="T36" s="2"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>1974</v>
       </c>
@@ -5011,7 +5017,7 @@
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>1975</v>
       </c>
@@ -5043,7 +5049,7 @@
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>1976</v>
       </c>
@@ -5075,7 +5081,7 @@
       <c r="S39" s="2"/>
       <c r="T39" s="2"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>1977</v>
       </c>
@@ -5107,7 +5113,7 @@
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>1978</v>
       </c>
@@ -5139,7 +5145,7 @@
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>1979</v>
       </c>
@@ -5171,7 +5177,7 @@
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>1980</v>
       </c>
@@ -5203,7 +5209,7 @@
       <c r="S43" s="2"/>
       <c r="T43" s="2"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>1981</v>
       </c>
@@ -5235,7 +5241,7 @@
       <c r="S44" s="2"/>
       <c r="T44" s="2"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
         <v>1982</v>
       </c>
@@ -5267,7 +5273,7 @@
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>1983</v>
       </c>
@@ -5299,7 +5305,7 @@
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>1984</v>
       </c>
@@ -5331,7 +5337,7 @@
       <c r="S47" s="2"/>
       <c r="T47" s="2"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <v>1985</v>
       </c>
@@ -5363,7 +5369,7 @@
       <c r="S48" s="2"/>
       <c r="T48" s="2"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
         <v>1986</v>
       </c>
@@ -5395,7 +5401,7 @@
       <c r="S49" s="2"/>
       <c r="T49" s="2"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="7">
         <v>1987</v>
       </c>
@@ -5427,7 +5433,7 @@
       <c r="S50" s="2"/>
       <c r="T50" s="2"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
         <v>1988</v>
       </c>
@@ -5459,7 +5465,7 @@
       <c r="S51" s="2"/>
       <c r="T51" s="2"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
         <v>1989</v>
       </c>
@@ -5491,7 +5497,7 @@
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>1990</v>
       </c>
@@ -5523,7 +5529,7 @@
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
         <v>1991</v>
       </c>
@@ -5555,7 +5561,7 @@
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <v>1992</v>
       </c>
@@ -5587,7 +5593,7 @@
       <c r="S55" s="2"/>
       <c r="T55" s="2"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
         <v>1993</v>
       </c>
@@ -5619,7 +5625,7 @@
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
         <v>1994</v>
       </c>
@@ -5651,7 +5657,7 @@
       <c r="S57" s="2"/>
       <c r="T57" s="2"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
         <v>1995</v>
       </c>
@@ -5683,7 +5689,7 @@
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>1996</v>
       </c>
@@ -5715,7 +5721,7 @@
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <v>1997</v>
       </c>
@@ -5747,7 +5753,7 @@
       <c r="S60" s="2"/>
       <c r="T60" s="2"/>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>1998</v>
       </c>
@@ -5779,7 +5785,7 @@
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <v>1999</v>
       </c>
@@ -5811,7 +5817,7 @@
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>2000</v>
       </c>
@@ -5843,7 +5849,7 @@
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
     </row>
-    <row r="64" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="7">
         <v>2001</v>
       </c>
@@ -5875,7 +5881,7 @@
       <c r="S64" s="2"/>
       <c r="T64" s="2"/>
     </row>
-    <row r="65" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="7">
         <v>-9999</v>
       </c>
@@ -5909,7 +5915,7 @@
       <c r="S65" s="2"/>
       <c r="T65" s="2"/>
     </row>
-    <row r="66" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>255</v>
       </c>
@@ -5933,7 +5939,7 @@
       <c r="S66" s="2"/>
       <c r="T66" s="2"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>2</v>
       </c>
@@ -5963,7 +5969,7 @@
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>6</v>
       </c>
@@ -5993,7 +5999,7 @@
       <c r="S68" s="2"/>
       <c r="T68" s="2"/>
     </row>
-    <row r="69" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>141</v>
       </c>
@@ -6017,7 +6023,7 @@
       <c r="S69" s="2"/>
       <c r="T69" s="2"/>
     </row>
-    <row r="70" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="13" t="s">
         <v>80</v>
       </c>
@@ -6047,7 +6053,7 @@
       <c r="S70" s="2"/>
       <c r="T70" s="2"/>
     </row>
-    <row r="71" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="12">
         <v>1</v>
       </c>
@@ -6081,7 +6087,7 @@
       <c r="S71" s="2"/>
       <c r="T71" s="2"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A72" s="12">
         <v>2</v>
       </c>
@@ -6113,7 +6119,7 @@
       <c r="S72" s="2"/>
       <c r="T72" s="2"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A73" s="12">
         <v>3</v>
       </c>
@@ -6145,7 +6151,7 @@
       <c r="S73" s="2"/>
       <c r="T73" s="2"/>
     </row>
-    <row r="74" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>13</v>
       </c>
@@ -6179,7 +6185,7 @@
       <c r="S74" s="2"/>
       <c r="T74" s="2"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" s="7">
         <v>1977</v>
       </c>
@@ -6213,7 +6219,7 @@
       <c r="S75" s="2"/>
       <c r="T75" s="2"/>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A76" s="7">
         <v>1980</v>
       </c>
@@ -6247,7 +6253,7 @@
       <c r="S76" s="2"/>
       <c r="T76" s="2"/>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A77" s="7">
         <v>1983</v>
       </c>
@@ -6281,7 +6287,7 @@
       <c r="S77" s="2"/>
       <c r="T77" s="2"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A78" s="7">
         <v>1986</v>
       </c>
@@ -6315,7 +6321,7 @@
       <c r="S78" s="2"/>
       <c r="T78" s="2"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A79" s="7">
         <v>1989</v>
       </c>
@@ -6349,7 +6355,7 @@
       <c r="S79" s="2"/>
       <c r="T79" s="2"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A80" s="7">
         <v>1992</v>
       </c>
@@ -6383,7 +6389,7 @@
       <c r="S80" s="2"/>
       <c r="T80" s="2"/>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A81" s="7">
         <v>1995</v>
       </c>
@@ -6417,7 +6423,7 @@
       <c r="S81" s="2"/>
       <c r="T81" s="2"/>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A82" s="7">
         <v>1998</v>
       </c>
@@ -6451,7 +6457,7 @@
       <c r="S82" s="2"/>
       <c r="T82" s="2"/>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" s="7">
         <v>2001</v>
       </c>
@@ -6485,7 +6491,7 @@
       <c r="S83" s="2"/>
       <c r="T83" s="2"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" s="7">
         <v>1990</v>
       </c>
@@ -6519,7 +6525,7 @@
       <c r="S84" s="2"/>
       <c r="T84" s="2"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A85" s="7">
         <v>1991</v>
       </c>
@@ -6553,7 +6559,7 @@
       <c r="S85" s="2"/>
       <c r="T85" s="2"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A86" s="7">
         <v>1992</v>
       </c>
@@ -6587,7 +6593,7 @@
       <c r="S86" s="2"/>
       <c r="T86" s="2"/>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A87" s="7">
         <v>1993</v>
       </c>
@@ -6621,7 +6627,7 @@
       <c r="S87" s="2"/>
       <c r="T87" s="2"/>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A88" s="7">
         <v>1994</v>
       </c>
@@ -6655,7 +6661,7 @@
       <c r="S88" s="2"/>
       <c r="T88" s="2"/>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A89" s="7">
         <v>1995</v>
       </c>
@@ -6689,7 +6695,7 @@
       <c r="S89" s="2"/>
       <c r="T89" s="2"/>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A90" s="7">
         <v>1996</v>
       </c>
@@ -6723,7 +6729,7 @@
       <c r="S90" s="2"/>
       <c r="T90" s="2"/>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A91" s="7">
         <v>1997</v>
       </c>
@@ -6757,7 +6763,7 @@
       <c r="S91" s="2"/>
       <c r="T91" s="2"/>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A92" s="7">
         <v>1998</v>
       </c>
@@ -6791,7 +6797,7 @@
       <c r="S92" s="2"/>
       <c r="T92" s="2"/>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A93" s="7">
         <v>1999</v>
       </c>
@@ -6825,7 +6831,7 @@
       <c r="S93" s="2"/>
       <c r="T93" s="2"/>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A94" s="7">
         <v>2000</v>
       </c>
@@ -6859,7 +6865,7 @@
       <c r="S94" s="2"/>
       <c r="T94" s="2"/>
     </row>
-    <row r="95" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A95" s="7">
         <v>2001</v>
       </c>
@@ -6893,7 +6899,7 @@
       <c r="S95" s="2"/>
       <c r="T95" s="2"/>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A96" s="7">
         <v>-9999</v>
       </c>
@@ -6927,7 +6933,7 @@
       <c r="S96" s="2"/>
       <c r="T96" s="2"/>
     </row>
-    <row r="97" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>195</v>
       </c>
@@ -6951,7 +6957,7 @@
       <c r="S97" s="2"/>
       <c r="T97" s="2"/>
     </row>
-    <row r="98" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A98" s="7">
         <v>0</v>
       </c>
@@ -6979,7 +6985,7 @@
       <c r="S98" s="2"/>
       <c r="T98" s="2"/>
     </row>
-    <row r="99" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>195</v>
       </c>
@@ -7003,7 +7009,7 @@
       <c r="S99" s="2"/>
       <c r="T99" s="2"/>
     </row>
-    <row r="100" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A100" s="7">
         <v>0</v>
       </c>
@@ -7031,7 +7037,7 @@
       <c r="S100" s="2"/>
       <c r="T100" s="2"/>
     </row>
-    <row r="101" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>195</v>
       </c>
@@ -7055,7 +7061,7 @@
       <c r="S101" s="2"/>
       <c r="T101" s="2"/>
     </row>
-    <row r="102" spans="1:23" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:23" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A102" s="60" t="s">
         <v>256</v>
       </c>
@@ -7082,7 +7088,7 @@
       <c r="V102" s="63"/>
       <c r="W102" s="64"/>
     </row>
-    <row r="103" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>257</v>
       </c>
@@ -7106,7 +7112,7 @@
       <c r="S103" s="2"/>
       <c r="T103" s="2"/>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A104" s="7">
         <v>2</v>
       </c>
@@ -7132,7 +7138,7 @@
       <c r="S104" s="2"/>
       <c r="T104" s="2"/>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A105" s="7">
         <v>2</v>
       </c>
@@ -7158,7 +7164,7 @@
       <c r="S105" s="2"/>
       <c r="T105" s="2"/>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A106" s="7">
         <v>10</v>
       </c>
@@ -7184,7 +7190,7 @@
       <c r="S106" s="2"/>
       <c r="T106" s="2"/>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A107" s="7">
         <v>94</v>
       </c>
@@ -7210,7 +7216,7 @@
       <c r="S107" s="2"/>
       <c r="T107" s="2"/>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A108" s="7">
         <v>1</v>
       </c>
@@ -7236,7 +7242,7 @@
       <c r="S108" s="2"/>
       <c r="T108" s="2"/>
     </row>
-    <row r="109" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>106</v>
       </c>
@@ -7260,7 +7266,7 @@
       <c r="S109" s="2"/>
       <c r="T109" s="2"/>
     </row>
-    <row r="110" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>107</v>
       </c>
@@ -7284,7 +7290,7 @@
       <c r="S110" s="2"/>
       <c r="T110" s="2"/>
     </row>
-    <row r="111" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>108</v>
       </c>
@@ -7308,7 +7314,7 @@
       <c r="S111" s="2"/>
       <c r="T111" s="2"/>
     </row>
-    <row r="112" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>109</v>
       </c>
@@ -7332,7 +7338,7 @@
       <c r="S112" s="2"/>
       <c r="T112" s="2"/>
     </row>
-    <row r="113" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>117</v>
       </c>
@@ -7356,7 +7362,7 @@
       <c r="S113" s="2"/>
       <c r="T113" s="2"/>
     </row>
-    <row r="114" spans="1:56" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:56" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>118</v>
       </c>
@@ -7380,7 +7386,7 @@
       <c r="S114" s="2"/>
       <c r="T114" s="2"/>
     </row>
-    <row r="115" spans="1:56" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:56" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>268</v>
       </c>
@@ -7406,7 +7412,7 @@
       <c r="S115" s="2"/>
       <c r="T115" s="2"/>
     </row>
-    <row r="116" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>132</v>
       </c>
@@ -7430,7 +7436,7 @@
       <c r="S116" s="2"/>
       <c r="T116" s="2"/>
     </row>
-    <row r="117" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>261</v>
       </c>
@@ -7466,7 +7472,7 @@
       <c r="S117" s="2"/>
       <c r="T117" s="2"/>
     </row>
-    <row r="118" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="7">
         <v>0</v>
       </c>
@@ -7504,7 +7510,7 @@
       <c r="S118" s="2"/>
       <c r="T118" s="2"/>
     </row>
-    <row r="119" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A119" s="7">
         <v>0</v>
       </c>
@@ -7542,7 +7548,7 @@
       <c r="S119" s="2"/>
       <c r="T119" s="2"/>
     </row>
-    <row r="120" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A120" s="7">
         <v>0</v>
       </c>
@@ -7580,7 +7586,7 @@
       <c r="S120" s="2"/>
       <c r="T120" s="2"/>
     </row>
-    <row r="121" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A121" s="7">
         <v>25</v>
       </c>
@@ -7606,7 +7612,7 @@
       <c r="S121" s="2"/>
       <c r="T121" s="2"/>
     </row>
-    <row r="122" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>76</v>
       </c>
@@ -7630,7 +7636,7 @@
       <c r="S122" s="2"/>
       <c r="T122" s="2"/>
     </row>
-    <row r="123" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A123" s="7">
         <v>26</v>
       </c>
@@ -7707,7 +7713,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="124" spans="1:56" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:56" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>17</v>
       </c>
@@ -7781,7 +7787,7 @@
       <c r="BC124" s="22"/>
       <c r="BD124" s="22"/>
     </row>
-    <row r="125" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A125" s="7">
         <v>1971</v>
       </c>
@@ -7951,7 +7957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A126" s="7">
         <v>1972</v>
       </c>
@@ -8121,7 +8127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A127" s="7">
         <v>1973</v>
       </c>
@@ -8291,7 +8297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A128" s="7">
         <v>1974</v>
       </c>
@@ -8461,7 +8467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A129" s="7">
         <v>1975</v>
       </c>
@@ -8631,7 +8637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A130" s="7">
         <v>1976</v>
       </c>
@@ -8801,7 +8807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A131" s="7">
         <v>1977</v>
       </c>
@@ -8971,7 +8977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A132" s="7">
         <v>1978</v>
       </c>
@@ -9141,7 +9147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A133" s="7">
         <v>1979</v>
       </c>
@@ -9311,7 +9317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A134" s="7">
         <v>1980</v>
       </c>
@@ -9481,7 +9487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A135" s="7">
         <v>1981</v>
       </c>
@@ -9651,7 +9657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A136" s="7">
         <v>1982</v>
       </c>
@@ -9821,7 +9827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A137" s="7">
         <v>1983</v>
       </c>
@@ -9991,7 +9997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A138" s="7">
         <v>1984</v>
       </c>
@@ -10161,7 +10167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A139" s="7">
         <v>1985</v>
       </c>
@@ -10331,7 +10337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A140" s="7">
         <v>1986</v>
       </c>
@@ -10501,7 +10507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A141" s="7">
         <v>1987</v>
       </c>
@@ -10671,7 +10677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A142" s="7">
         <v>1988</v>
       </c>
@@ -10841,7 +10847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A143" s="7">
         <v>1989</v>
       </c>
@@ -11011,7 +11017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A144" s="7">
         <v>1990</v>
       </c>
@@ -11181,7 +11187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A145" s="7">
         <v>1991</v>
       </c>
@@ -11351,7 +11357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A146" s="7">
         <v>1992</v>
       </c>
@@ -11521,7 +11527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A147" s="7">
         <v>1993</v>
       </c>
@@ -11691,7 +11697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A148" s="7">
         <v>1994</v>
       </c>
@@ -11861,7 +11867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A149" s="7">
         <v>1995</v>
       </c>
@@ -12031,7 +12037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A150" s="7">
         <v>1996</v>
       </c>
@@ -12201,7 +12207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A151" s="7">
         <v>1997</v>
       </c>
@@ -12371,7 +12377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A152" s="7">
         <v>1998</v>
       </c>
@@ -12541,7 +12547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A153" s="7">
         <v>1999</v>
       </c>
@@ -12711,7 +12717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A154" s="7">
         <v>2000</v>
       </c>
@@ -12881,7 +12887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A155" s="7">
         <v>2001</v>
       </c>
@@ -13051,7 +13057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A156" s="7">
         <v>1977</v>
       </c>
@@ -13221,7 +13227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A157" s="7">
         <v>1980</v>
       </c>
@@ -13391,7 +13397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A158" s="7">
         <v>1983</v>
       </c>
@@ -13561,7 +13567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A159" s="7">
         <v>1986</v>
       </c>
@@ -13731,7 +13737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A160" s="7">
         <v>1989</v>
       </c>
@@ -13901,7 +13907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A161" s="7">
         <v>1992</v>
       </c>
@@ -14071,7 +14077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A162" s="7">
         <v>1995</v>
       </c>
@@ -14241,7 +14247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A163" s="7">
         <v>1998</v>
       </c>
@@ -14411,7 +14417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A164" s="7">
         <v>2001</v>
       </c>
@@ -14581,7 +14587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A165" s="7">
         <v>1990</v>
       </c>
@@ -14751,7 +14757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A166" s="7">
         <v>1991</v>
       </c>
@@ -14921,7 +14927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A167" s="7">
         <v>1992</v>
       </c>
@@ -15091,7 +15097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A168" s="7">
         <v>1993</v>
       </c>
@@ -15261,7 +15267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A169" s="7">
         <v>1994</v>
       </c>
@@ -15431,7 +15437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A170" s="7">
         <v>1995</v>
       </c>
@@ -15601,7 +15607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A171" s="7">
         <v>1996</v>
       </c>
@@ -15771,7 +15777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A172" s="7">
         <v>1997</v>
       </c>
@@ -15941,7 +15947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A173" s="7">
         <v>1998</v>
       </c>
@@ -16111,7 +16117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A174" s="7">
         <v>1999</v>
       </c>
@@ -16281,7 +16287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A175" s="7">
         <v>-9999</v>
       </c>
@@ -16451,7 +16457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:56" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>195</v>
       </c>
@@ -16498,7 +16504,7 @@
       <c r="AP176" s="2"/>
       <c r="AQ176" s="2"/>
     </row>
-    <row r="177" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A177" s="7">
         <v>17</v>
       </c>
@@ -16547,7 +16553,7 @@
       <c r="AP177" s="2"/>
       <c r="AQ177" s="2"/>
     </row>
-    <row r="178" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>77</v>
       </c>
@@ -16594,7 +16600,7 @@
       <c r="AP178" s="2"/>
       <c r="AQ178" s="2"/>
     </row>
-    <row r="179" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A179" s="7">
         <v>1</v>
       </c>
@@ -16673,7 +16679,7 @@
       <c r="AP179" s="2"/>
       <c r="AQ179" s="2"/>
     </row>
-    <row r="180" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A180" s="7">
         <v>2</v>
       </c>
@@ -16722,7 +16728,7 @@
       <c r="AP180" s="2"/>
       <c r="AQ180" s="2"/>
     </row>
-    <row r="181" spans="1:43" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:43" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -16767,7 +16773,7 @@
       <c r="AP181" s="2"/>
       <c r="AQ181" s="2"/>
     </row>
-    <row r="182" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -16812,7 +16818,7 @@
       <c r="AP182" s="2"/>
       <c r="AQ182" s="2"/>
     </row>
-    <row r="183" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -16857,7 +16863,7 @@
       <c r="AP183" s="2"/>
       <c r="AQ183" s="2"/>
     </row>
-    <row r="184" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -16902,7 +16908,7 @@
       <c r="AP184" s="2"/>
       <c r="AQ184" s="2"/>
     </row>
-    <row r="185" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" s="19" t="s">
         <v>166</v>
       </c>
@@ -16949,7 +16955,7 @@
       <c r="AP185" s="2"/>
       <c r="AQ185" s="2"/>
     </row>
-    <row r="186" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A186" s="7">
         <v>-1</v>
       </c>
@@ -17076,7 +17082,7 @@
       <c r="AP186" s="2"/>
       <c r="AQ186" s="2"/>
     </row>
-    <row r="187" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A187" s="7">
         <v>1E-3</v>
       </c>
@@ -17203,7 +17209,7 @@
       <c r="AP187" s="2"/>
       <c r="AQ187" s="2"/>
     </row>
-    <row r="188" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="19" t="s">
         <v>167</v>
       </c>
@@ -17250,7 +17256,7 @@
       <c r="AP188" s="2"/>
       <c r="AQ188" s="2"/>
     </row>
-    <row r="189" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A189" s="7">
         <v>0.5</v>
       </c>
@@ -17377,7 +17383,7 @@
       <c r="AP189" s="2"/>
       <c r="AQ189" s="2"/>
     </row>
-    <row r="190" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A190" s="7">
         <v>0.5</v>
       </c>
@@ -17504,7 +17510,7 @@
       <c r="AP190" s="2"/>
       <c r="AQ190" s="2"/>
     </row>
-    <row r="191" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>195</v>
       </c>
@@ -17551,7 +17557,7 @@
       <c r="AP191" s="2"/>
       <c r="AQ191" s="2"/>
     </row>
-    <row r="192" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>106</v>
       </c>
@@ -17598,7 +17604,7 @@
       <c r="AP192" s="2"/>
       <c r="AQ192" s="2"/>
     </row>
-    <row r="193" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>107</v>
       </c>
@@ -17645,7 +17651,7 @@
       <c r="AP193" s="2"/>
       <c r="AQ193" s="2"/>
     </row>
-    <row r="194" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>108</v>
       </c>
@@ -17692,7 +17698,7 @@
       <c r="AP194" s="2"/>
       <c r="AQ194" s="2"/>
     </row>
-    <row r="195" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>109</v>
       </c>
@@ -17739,7 +17745,7 @@
       <c r="AP195" s="2"/>
       <c r="AQ195" s="2"/>
     </row>
-    <row r="196" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>117</v>
       </c>
@@ -17786,7 +17792,7 @@
       <c r="AP196" s="2"/>
       <c r="AQ196" s="2"/>
     </row>
-    <row r="197" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>118</v>
       </c>
@@ -17833,7 +17839,7 @@
       <c r="AP197" s="2"/>
       <c r="AQ197" s="2"/>
     </row>
-    <row r="198" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>119</v>
       </c>
@@ -17880,7 +17886,7 @@
       <c r="AP198" s="2"/>
       <c r="AQ198" s="2"/>
     </row>
-    <row r="199" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>132</v>
       </c>
@@ -17927,7 +17933,7 @@
       <c r="AP199" s="2"/>
       <c r="AQ199" s="2"/>
     </row>
-    <row r="200" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A200" s="7">
         <v>0</v>
       </c>
@@ -17988,7 +17994,7 @@
       <c r="AP200" s="2"/>
       <c r="AQ200" s="2"/>
     </row>
-    <row r="201" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A201" s="7">
         <v>0</v>
       </c>
@@ -18049,7 +18055,7 @@
       <c r="AP201" s="2"/>
       <c r="AQ201" s="2"/>
     </row>
-    <row r="202" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A202" s="7">
         <v>0</v>
       </c>
@@ -18110,7 +18116,7 @@
       <c r="AP202" s="2"/>
       <c r="AQ202" s="2"/>
     </row>
-    <row r="203" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A203" s="7">
         <v>1</v>
       </c>
@@ -18159,7 +18165,7 @@
       <c r="AP203" s="2"/>
       <c r="AQ203" s="2"/>
     </row>
-    <row r="204" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A204" s="7">
         <v>40</v>
       </c>
@@ -18208,7 +18214,7 @@
       <c r="AP204" s="2"/>
       <c r="AQ204" s="2"/>
     </row>
-    <row r="205" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>79</v>
       </c>
@@ -18255,7 +18261,7 @@
       <c r="AP205" s="2"/>
       <c r="AQ205" s="2"/>
     </row>
-    <row r="206" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:43" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>17</v>
       </c>
@@ -18320,7 +18326,7 @@
       <c r="AP206" s="2"/>
       <c r="AQ206" s="2"/>
     </row>
-    <row r="207" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A207" s="7">
         <v>1971</v>
       </c>
@@ -18451,7 +18457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="208" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A208" s="7">
         <v>1972</v>
       </c>
@@ -18582,7 +18588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A209" s="7">
         <v>1973</v>
       </c>
@@ -18713,7 +18719,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="210" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A210" s="7">
         <v>1974</v>
       </c>
@@ -18844,7 +18850,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="211" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A211" s="7">
         <v>1975</v>
       </c>
@@ -18975,7 +18981,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A212" s="7">
         <v>1976</v>
       </c>
@@ -19106,7 +19112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A213" s="7">
         <v>1977</v>
       </c>
@@ -19237,7 +19243,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A214" s="7">
         <v>1978</v>
       </c>
@@ -19368,7 +19374,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="215" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A215" s="7">
         <v>1979</v>
       </c>
@@ -19499,7 +19505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A216" s="7">
         <v>1980</v>
       </c>
@@ -19630,7 +19636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="217" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A217" s="7">
         <v>1981</v>
       </c>
@@ -19761,7 +19767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="218" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A218" s="7">
         <v>1982</v>
       </c>
@@ -19892,7 +19898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A219" s="7">
         <v>1983</v>
       </c>
@@ -20023,7 +20029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A220" s="7">
         <v>1984</v>
       </c>
@@ -20154,7 +20160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A221" s="7">
         <v>1985</v>
       </c>
@@ -20285,7 +20291,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A222" s="7">
         <v>1986</v>
       </c>
@@ -20416,7 +20422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A223" s="7">
         <v>1987</v>
       </c>
@@ -20547,7 +20553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A224" s="7">
         <v>1988</v>
       </c>
@@ -20678,7 +20684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A225" s="7">
         <v>1989</v>
       </c>
@@ -20809,7 +20815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A226" s="7">
         <v>1990</v>
       </c>
@@ -20940,7 +20946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A227" s="7">
         <v>1991</v>
       </c>
@@ -21071,7 +21077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A228" s="7">
         <v>1992</v>
       </c>
@@ -21202,7 +21208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A229" s="7">
         <v>1993</v>
       </c>
@@ -21333,7 +21339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A230" s="7">
         <v>1994</v>
       </c>
@@ -21464,7 +21470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A231" s="7">
         <v>1995</v>
       </c>
@@ -21595,7 +21601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A232" s="7">
         <v>1996</v>
       </c>
@@ -21726,7 +21732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A233" s="7">
         <v>1997</v>
       </c>
@@ -21857,7 +21863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A234" s="7">
         <v>1998</v>
       </c>
@@ -21988,7 +21994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A235" s="7">
         <v>1999</v>
       </c>
@@ -22119,7 +22125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A236" s="7">
         <v>2000</v>
       </c>
@@ -22250,7 +22256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A237" s="7">
         <v>2001</v>
       </c>
@@ -22381,7 +22387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A238" s="7">
         <v>1977</v>
       </c>
@@ -22512,7 +22518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A239" s="7">
         <v>1980</v>
       </c>
@@ -22643,7 +22649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A240" s="7">
         <v>1983</v>
       </c>
@@ -22774,7 +22780,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A241" s="7">
         <v>1986</v>
       </c>
@@ -22905,7 +22911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A242" s="7">
         <v>1989</v>
       </c>
@@ -23036,7 +23042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A243" s="7">
         <v>1992</v>
       </c>
@@ -23167,7 +23173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A244" s="7">
         <v>1995</v>
       </c>
@@ -23298,7 +23304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A245" s="7">
         <v>1998</v>
       </c>
@@ -23429,7 +23435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:44" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A246" s="7">
         <v>2001</v>
       </c>
@@ -23560,7 +23566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A247" s="7">
         <v>-9999</v>
       </c>
@@ -23691,7 +23697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A248" s="2" t="s">
         <v>195</v>
       </c>
@@ -23739,7 +23745,7 @@
       <c r="AQ248" s="2"/>
       <c r="AR248" s="16"/>
     </row>
-    <row r="249" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A249" s="7">
         <v>0</v>
       </c>
@@ -23791,7 +23797,7 @@
       <c r="AQ249" s="2"/>
       <c r="AR249" s="16"/>
     </row>
-    <row r="250" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A250" s="2" t="s">
         <v>195</v>
       </c>
@@ -23839,7 +23845,7 @@
       <c r="AQ250" s="2"/>
       <c r="AR250" s="16"/>
     </row>
-    <row r="251" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A251" s="7">
         <v>0</v>
       </c>
@@ -23891,7 +23897,7 @@
       <c r="AQ251" s="2"/>
       <c r="AR251" s="16"/>
     </row>
-    <row r="252" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A252" s="2" t="s">
         <v>195</v>
       </c>
@@ -23939,7 +23945,7 @@
       <c r="AQ252" s="2"/>
       <c r="AR252" s="16"/>
     </row>
-    <row r="253" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A253" s="7">
         <v>0</v>
       </c>
@@ -23991,7 +23997,7 @@
       <c r="AQ253" s="2"/>
       <c r="AR253" s="16"/>
     </row>
-    <row r="254" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A254" s="2" t="s">
         <v>195</v>
       </c>
@@ -24039,7 +24045,7 @@
       <c r="AQ254" s="2"/>
       <c r="AR254" s="16"/>
     </row>
-    <row r="255" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A255" s="7">
         <v>0</v>
       </c>
@@ -24090,7 +24096,7 @@
       <c r="AP255" s="2"/>
       <c r="AQ255" s="2"/>
     </row>
-    <row r="256" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:44" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A256" s="2" t="s">
         <v>195</v>
       </c>
@@ -24137,7 +24143,7 @@
       <c r="AP256" s="2"/>
       <c r="AQ256" s="2"/>
     </row>
-    <row r="257" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A257" s="7">
         <v>0</v>
       </c>
@@ -24188,7 +24194,7 @@
       <c r="AP257" s="2"/>
       <c r="AQ257" s="2"/>
     </row>
-    <row r="258" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A258" s="2" t="s">
         <v>195</v>
       </c>
@@ -24235,7 +24241,7 @@
       <c r="AP258" s="2"/>
       <c r="AQ258" s="2"/>
     </row>
-    <row r="259" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A259" s="7">
         <v>0</v>
       </c>
@@ -48671,7 +48677,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="260" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
         <v>195</v>
       </c>
@@ -48718,7 +48724,7 @@
       <c r="AP260" s="2"/>
       <c r="AQ260" s="2"/>
     </row>
-    <row r="261" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" x14ac:dyDescent="0.3">
       <c r="A261" s="7">
         <v>999</v>
       </c>
@@ -48767,7 +48773,7 @@
       <c r="AP261" s="2"/>
       <c r="AQ261" s="2"/>
     </row>
-    <row r="262" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" x14ac:dyDescent="0.3">
       <c r="A262" s="2"/>
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
@@ -48812,7 +48818,7 @@
       <c r="AP262" s="2"/>
       <c r="AQ262" s="2"/>
     </row>
-    <row r="263" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:1022 1025:2046 2049:3070 3073:4094 4097:5118 5121:6142 6145:7166 7169:8190 8193:9214 9217:10238 10241:11262 11265:12286 12289:13310 13313:14334 14337:15358 15361:16382" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
         <v>258</v>
       </c>
@@ -48883,24 +48889,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:13" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -48919,9 +48927,9 @@
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>95</v>
+        <v>271</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -48936,7 +48944,7 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>168</v>
       </c>
@@ -48953,7 +48961,7 @@
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>96</v>
       </c>
@@ -48970,7 +48978,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>97</v>
       </c>
@@ -48987,7 +48995,7 @@
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>169</v>
       </c>
@@ -49004,7 +49012,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>170</v>
       </c>
@@ -49021,7 +49029,7 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>171</v>
       </c>
@@ -49038,7 +49046,7 @@
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>1</v>
       </c>
@@ -49067,7 +49075,7 @@
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>3</v>
       </c>
@@ -49096,7 +49104,7 @@
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>3</v>
       </c>
@@ -49125,7 +49133,7 @@
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -49134,7 +49142,7 @@
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -49143,16 +49151,26 @@
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
+    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="60" t="s">
+        <v>272</v>
+      </c>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="63"/>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="63"/>
+      <c r="L19" s="63"/>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="64"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -49161,7 +49179,7 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -49182,14 +49200,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="3" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="2" max="3" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>197</v>
       </c>
@@ -49197,8 +49215,8 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -49214,7 +49232,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -49230,7 +49248,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>141</v>
       </c>
@@ -49240,7 +49258,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>80</v>
       </c>
@@ -49256,7 +49274,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>1</v>
       </c>
@@ -49274,7 +49292,7 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>2</v>
       </c>
@@ -49292,7 +49310,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="20">
         <v>3</v>
       </c>
@@ -49310,7 +49328,7 @@
       </c>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>194</v>
       </c>
@@ -49330,7 +49348,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>1977</v>
       </c>
@@ -49350,7 +49368,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>1980</v>
       </c>
@@ -49370,7 +49388,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>1983</v>
       </c>
@@ -49390,7 +49408,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>1986</v>
       </c>
@@ -49410,7 +49428,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>1989</v>
       </c>
@@ -49430,7 +49448,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>1992</v>
       </c>
@@ -49450,7 +49468,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>1995</v>
       </c>
@@ -49470,7 +49488,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>1977</v>
       </c>
@@ -49490,7 +49508,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>1980</v>
       </c>
@@ -49510,7 +49528,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>1983</v>
       </c>
@@ -49530,7 +49548,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>1986</v>
       </c>
@@ -49550,7 +49568,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="7">
         <v>1989</v>
       </c>
@@ -49570,7 +49588,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="28">
         <v>1977</v>
       </c>
@@ -49590,7 +49608,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="32">
         <v>2001</v>
       </c>
@@ -49625,21 +49643,21 @@
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:29" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:29" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" s="18" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
       <c r="J3" s="37"/>
       <c r="K3" s="37"/>
@@ -49662,7 +49680,7 @@
       <c r="AB3"/>
       <c r="AC3"/>
     </row>
-    <row r="4" spans="1:29" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" ht="21" x14ac:dyDescent="0.4">
       <c r="J4" s="37"/>
       <c r="K4" s="37"/>
       <c r="L4" s="37"/>
@@ -49679,7 +49697,7 @@
       <c r="W4" s="37"/>
       <c r="X4" s="37"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="J5" s="37"/>
       <c r="K5" s="37"/>
       <c r="L5" s="37"/>
@@ -49696,7 +49714,7 @@
       <c r="W5" s="37"/>
       <c r="X5" s="37"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -49726,7 +49744,7 @@
       <c r="W6" s="37"/>
       <c r="X6" s="37"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>181</v>
       </c>
@@ -49754,7 +49772,7 @@
       <c r="W7" s="37"/>
       <c r="X7" s="37"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>172</v>
       </c>
@@ -49782,7 +49800,7 @@
       <c r="W8" s="37"/>
       <c r="X8" s="37"/>
     </row>
-    <row r="9" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>178</v>
       </c>
@@ -49815,7 +49833,7 @@
       <c r="AB9"/>
       <c r="AC9"/>
     </row>
-    <row r="10" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>177</v>
       </c>
@@ -49848,7 +49866,7 @@
       <c r="AB10"/>
       <c r="AC10"/>
     </row>
-    <row r="11" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>176</v>
       </c>
@@ -49881,7 +49899,7 @@
       <c r="AB11"/>
       <c r="AC11"/>
     </row>
-    <row r="12" spans="1:29" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>179</v>
       </c>
@@ -49914,7 +49932,7 @@
       <c r="AB12"/>
       <c r="AC12"/>
     </row>
-    <row r="13" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
         <v>173</v>
       </c>
@@ -49948,7 +49966,7 @@
       <c r="W13" s="37"/>
       <c r="X13" s="37"/>
     </row>
-    <row r="14" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>1</v>
       </c>
@@ -49984,7 +50002,7 @@
       <c r="W14" s="37"/>
       <c r="X14" s="37"/>
     </row>
-    <row r="15" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -50024,7 +50042,7 @@
       <c r="W15" s="37"/>
       <c r="X15" s="37"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>1994</v>
       </c>
@@ -50062,7 +50080,7 @@
       <c r="W16" s="37"/>
       <c r="X16" s="37"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>1995</v>
       </c>
@@ -50100,7 +50118,7 @@
       <c r="W17" s="37"/>
       <c r="X17" s="37"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>1996</v>
       </c>
@@ -50138,7 +50156,7 @@
       <c r="W18" s="37"/>
       <c r="X18" s="37"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>1997</v>
       </c>
@@ -50165,7 +50183,7 @@
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>1998</v>
       </c>
@@ -50192,7 +50210,7 @@
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>-9999</v>
       </c>
@@ -50219,8 +50237,8 @@
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
     </row>
-    <row r="22" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>1</v>
       </c>
@@ -50234,7 +50252,7 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>181</v>
       </c>
@@ -50246,7 +50264,7 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>172</v>
       </c>
@@ -50258,7 +50276,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>178</v>
       </c>
@@ -50270,45 +50288,45 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>177</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="72" t="s">
+      <c r="E30" s="73" t="s">
         <v>206</v>
       </c>
-      <c r="F30" s="73"/>
-      <c r="G30" s="74"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="75"/>
       <c r="H30" s="47"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="77"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="78"/>
       <c r="H31" s="47"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="76"/>
-      <c r="G32" s="77"/>
+      <c r="E32" s="76"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="78"/>
       <c r="H32" s="47"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>173</v>
       </c>
@@ -50319,12 +50337,12 @@
         <v>175</v>
       </c>
       <c r="D33" s="2"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="76"/>
-      <c r="G33" s="77"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="78"/>
       <c r="H33" s="47"/>
     </row>
-    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>1</v>
       </c>
@@ -50337,12 +50355,12 @@
       <c r="D34" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E34" s="78"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="80"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="81"/>
       <c r="H34" s="47"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>13</v>
       </c>
@@ -50364,7 +50382,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>1994</v>
       </c>
@@ -50386,7 +50404,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="7">
         <v>1995</v>
       </c>
@@ -50408,7 +50426,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
         <v>1996</v>
       </c>
@@ -50430,7 +50448,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
         <v>1997</v>
       </c>
@@ -50452,7 +50470,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>1998</v>
       </c>
@@ -50474,7 +50492,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>-9999</v>
       </c>
@@ -50496,7 +50514,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>1</v>
       </c>
@@ -50510,7 +50528,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>181</v>
       </c>
@@ -50522,7 +50540,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>172</v>
       </c>
@@ -50534,7 +50552,7 @@
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>178</v>
       </c>
@@ -50546,7 +50564,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>177</v>
       </c>
@@ -50558,7 +50576,7 @@
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>176</v>
       </c>
@@ -50570,7 +50588,7 @@
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>179</v>
       </c>
@@ -50582,7 +50600,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
         <v>173</v>
       </c>
@@ -50598,7 +50616,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="12">
         <v>1</v>
       </c>
@@ -50616,7 +50634,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>13</v>
       </c>
@@ -50638,7 +50656,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
         <v>1994</v>
       </c>
@@ -50660,7 +50678,7 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
         <v>1995</v>
       </c>
@@ -50682,7 +50700,7 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
         <v>1996</v>
       </c>
@@ -50704,7 +50722,7 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>1997</v>
       </c>
@@ -50726,7 +50744,7 @@
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
         <v>1998</v>
       </c>
@@ -50748,7 +50766,7 @@
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>-9999</v>
       </c>
@@ -50786,12 +50804,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>213</v>
       </c>
@@ -50799,8 +50817,8 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -50820,7 +50838,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>30</v>
       </c>
@@ -50840,7 +50858,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>183</v>
       </c>
@@ -50860,7 +50878,7 @@
       <c r="M8" s="49"/>
       <c r="N8" s="50"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -50894,7 +50912,7 @@
       <c r="M9" s="52"/>
       <c r="N9" s="53"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>1994</v>
       </c>
@@ -50928,7 +50946,7 @@
       <c r="M10" s="52"/>
       <c r="N10" s="53"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>1995</v>
       </c>
@@ -50962,7 +50980,7 @@
       <c r="M11" s="55"/>
       <c r="N11" s="56"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>1996</v>
       </c>
@@ -50994,7 +51012,7 @@
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>1997</v>
       </c>
@@ -51026,7 +51044,7 @@
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>1998</v>
       </c>
@@ -51058,7 +51076,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>-9999</v>
       </c>
@@ -51102,9 +51120,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:77" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:77" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>214</v>
       </c>
@@ -51112,7 +51130,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:77" x14ac:dyDescent="0.3">
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
@@ -51188,7 +51206,7 @@
       <c r="BV3" s="18"/>
       <c r="BW3" s="18"/>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>4</v>
       </c>
@@ -51271,7 +51289,7 @@
       <c r="BX4" s="2"/>
       <c r="BY4" s="2"/>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -51352,7 +51370,7 @@
       <c r="BX5" s="2"/>
       <c r="BY5" s="2"/>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -51447,7 +51465,7 @@
       <c r="BX6" s="2"/>
       <c r="BY6" s="2"/>
     </row>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>1971</v>
       </c>
@@ -51676,7 +51694,7 @@
       <c r="BX7" s="2"/>
       <c r="BY7" s="2"/>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>1995</v>
       </c>
@@ -51905,7 +51923,7 @@
       <c r="BX8" s="2"/>
       <c r="BY8" s="2"/>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>1971</v>
       </c>
@@ -52134,7 +52152,7 @@
       <c r="BX9" s="2"/>
       <c r="BY9" s="2"/>
     </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>1995</v>
       </c>
@@ -52363,7 +52381,7 @@
       <c r="BX10" s="2"/>
       <c r="BY10" s="2"/>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:77" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>-9999</v>
       </c>
@@ -52609,14 +52627,14 @@
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>3</v>
       </c>
@@ -52631,7 +52649,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -52648,7 +52666,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>1980</v>
       </c>
@@ -52665,7 +52683,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>1981</v>
       </c>
@@ -52682,7 +52700,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>1982</v>
       </c>
@@ -52699,7 +52717,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>1983</v>
       </c>
@@ -52716,7 +52734,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>1984</v>
       </c>
@@ -52733,7 +52751,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>1980</v>
       </c>
@@ -52750,7 +52768,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>1981</v>
       </c>
@@ -52767,7 +52785,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>1982</v>
       </c>
@@ -52784,7 +52802,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>1983</v>
       </c>
@@ -52801,7 +52819,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>1984</v>
       </c>
@@ -52818,7 +52836,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>1980</v>
       </c>
@@ -52835,7 +52853,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>1981</v>
       </c>
@@ -52852,7 +52870,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>1982</v>
       </c>
@@ -52869,7 +52887,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>1983</v>
       </c>
@@ -52886,7 +52904,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="7">
         <v>1984</v>
       </c>
@@ -52903,7 +52921,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
         <v>-1</v>
       </c>
@@ -52922,7 +52940,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <v>-2</v>
       </c>
@@ -52941,7 +52959,7 @@
       <c r="H20" s="41"/>
       <c r="I20" s="57"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>-9999</v>
       </c>
@@ -52973,14 +52991,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -53015,7 +53033,7 @@
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>8</v>
       </c>
@@ -53052,7 +53070,7 @@
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>1</v>
       </c>
@@ -53089,7 +53107,7 @@
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -53126,7 +53144,7 @@
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>1.0000000000000001E-9</v>
       </c>
@@ -53163,7 +53181,7 @@
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>2</v>
       </c>
@@ -53200,7 +53218,7 @@
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>60</v>
       </c>
@@ -53233,7 +53251,7 @@
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>9.9999999999999995E-7</v>
       </c>
@@ -53280,7 +53298,7 @@
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>9.9999999999999995E-7</v>
       </c>
@@ -53333,7 +53351,7 @@
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>61</v>
       </c>
@@ -53366,7 +53384,7 @@
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>53</v>
       </c>
@@ -53413,7 +53431,7 @@
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>1</v>
       </c>
@@ -53490,7 +53508,7 @@
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>1</v>
       </c>
@@ -53567,7 +53585,7 @@
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>195</v>
       </c>
@@ -53600,7 +53618,7 @@
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>2</v>
       </c>
@@ -53689,7 +53707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <v>2</v>
       </c>

</xml_diff>